<commit_message>
Modified Test methods for Merchant Portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-merchant.xlsx
+++ b/Web/coyni/resources/TestScript-merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Merchant-Web\clone_Merchant_06_10_2022\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A5ED8D-472F-44F3-8DCA-D9945534D1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD510C8-3177-4B1F-B59B-33380566A572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16020" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -937,11 +937,6 @@
     <t>Exports</t>
   </si>
   <si>
-    <t>coyni.merchant.tests.TokenAccountTest,
-testExportSelectedTransactionToday,
--pheading</t>
-  </si>
-  <si>
     <t>Verify Exports Selected Today Transaction</t>
   </si>
   <si>
@@ -955,11 +950,6 @@
   </si>
   <si>
     <t>Verify Exports Selected LastMonth Transaction</t>
-  </si>
-  <si>
-    <t>coyni.merchant.tests.TokenAccountTest,
-testExportSelectedTransactionYesterday,
--pheading</t>
   </si>
   <si>
     <t>coyni.merchant.tests.TokenAccountTest,
@@ -1819,9 +1809,6 @@
   </si>
   <si>
     <t>Verify Without Generate Printable QR Code</t>
-  </si>
-  <si>
-    <t>15</t>
   </si>
   <si>
     <t>coyni.merchant.tests.MerchantSettingsTest,
@@ -2309,6 +2296,21 @@
 testWithdrawToUSDDeleteSignetAccount,
 -psignetNumber
 </t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.TokenAccountTest,
+testExportSelectedTransactionToday,
+-pheading,
+-pnotificationText</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.TokenAccountTest,
+testExportSelectedTransactionYesterday,
+-pheading,
+-pnotificationText</t>
   </si>
 </sst>
 </file>
@@ -2823,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,7 +2923,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -2948,12 +2950,12 @@
         <v>12</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="243.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -2974,12 +2976,12 @@
         <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -2997,15 +2999,15 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -3026,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
@@ -3052,7 +3054,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -3118,7 +3120,7 @@
     </row>
     <row r="11" spans="1:11" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
@@ -3139,7 +3141,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -3168,7 +3170,7 @@
         <v>14</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="18"/>
@@ -3205,7 +3207,7 @@
     </row>
     <row r="14" spans="1:11" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -3226,7 +3228,7 @@
         <v>14</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="18"/>
@@ -3290,7 +3292,7 @@
     </row>
     <row r="17" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
@@ -3311,7 +3313,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I17" s="6"/>
     </row>
@@ -3449,7 +3451,7 @@
     </row>
     <row r="23" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>26</v>
@@ -3470,7 +3472,7 @@
         <v>59</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
@@ -3522,7 +3524,7 @@
         <v>25</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>81</v>
@@ -3551,7 +3553,7 @@
         <v>25</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>93</v>
@@ -3580,7 +3582,7 @@
         <v>141</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>142</v>
@@ -3609,7 +3611,7 @@
         <v>121</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>143</v>
@@ -3638,7 +3640,7 @@
         <v>145</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>146</v>
@@ -3652,7 +3654,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>27</v>
@@ -3664,13 +3666,13 @@
         <v>11</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -3682,7 +3684,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>27</v>
@@ -3694,13 +3696,13 @@
         <v>11</v>
       </c>
       <c r="G31" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>237</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -3712,7 +3714,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>27</v>
@@ -3724,13 +3726,13 @@
         <v>11</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -3742,7 +3744,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>10</v>
@@ -3754,55 +3756,55 @@
         <v>19</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I34" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>27</v>
@@ -3814,19 +3816,19 @@
         <v>11</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>26</v>
@@ -3847,10 +3849,10 @@
         <v>116</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="J36" s="6"/>
     </row>
@@ -3877,7 +3879,7 @@
         <v>148</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>149</v>
@@ -3906,7 +3908,7 @@
         <v>150</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>172</v>
@@ -3935,7 +3937,7 @@
         <v>153</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>173</v>
@@ -3964,7 +3966,7 @@
         <v>158</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>171</v>
@@ -3993,7 +3995,7 @@
         <v>159</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>174</v>
@@ -4022,7 +4024,7 @@
         <v>155</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>170</v>
@@ -4051,7 +4053,7 @@
         <v>161</v>
       </c>
       <c r="H43" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>169</v>
@@ -4059,7 +4061,7 @@
     </row>
     <row r="44" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>26</v>
@@ -4077,13 +4079,13 @@
         <v>11</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H44" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4109,7 +4111,7 @@
         <v>163</v>
       </c>
       <c r="H45" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>164</v>
@@ -4138,7 +4140,7 @@
         <v>150</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>168</v>
@@ -4167,7 +4169,7 @@
         <v>158</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>167</v>
@@ -4196,7 +4198,7 @@
         <v>155</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>177</v>
@@ -4225,7 +4227,7 @@
         <v>153</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>178</v>
@@ -4254,7 +4256,7 @@
         <v>159</v>
       </c>
       <c r="H50" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I50" s="7" t="s">
         <v>180</v>
@@ -4283,7 +4285,7 @@
         <v>161</v>
       </c>
       <c r="H51" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>182</v>
@@ -4312,10 +4314,10 @@
         <v>192</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4341,21 +4343,21 @@
         <v>28</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D54" s="16" t="s">
         <v>27</v>
@@ -4367,13 +4369,13 @@
         <v>11</v>
       </c>
       <c r="G54" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="H54" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I54" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="H54" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>246</v>
       </c>
       <c r="J54" s="6"/>
     </row>
@@ -4400,10 +4402,10 @@
         <v>185</v>
       </c>
       <c r="H55" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4429,10 +4431,10 @@
         <v>184</v>
       </c>
       <c r="H56" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4458,10 +4460,10 @@
         <v>187</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4487,7 +4489,7 @@
         <v>189</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I58" s="14" t="s">
         <v>190</v>
@@ -4495,7 +4497,7 @@
     </row>
     <row r="59" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>26</v>
@@ -4516,15 +4518,15 @@
         <v>189</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>26</v>
@@ -4545,10 +4547,10 @@
         <v>189</v>
       </c>
       <c r="H60" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4574,7 +4576,7 @@
         <v>193</v>
       </c>
       <c r="H61" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I61" s="14" t="s">
         <v>202</v>
@@ -4603,7 +4605,7 @@
         <v>193</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I62" s="14" t="s">
         <v>201</v>
@@ -4611,7 +4613,7 @@
     </row>
     <row r="63" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>26</v>
@@ -4632,10 +4634,10 @@
         <v>193</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -4661,7 +4663,7 @@
         <v>193</v>
       </c>
       <c r="H64" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I64" s="14" t="s">
         <v>199</v>
@@ -4690,7 +4692,7 @@
         <v>193</v>
       </c>
       <c r="H65" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I65" s="14" t="s">
         <v>198</v>
@@ -4698,7 +4700,7 @@
     </row>
     <row r="66" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A66" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>26</v>
@@ -4719,15 +4721,15 @@
         <v>193</v>
       </c>
       <c r="H66" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" s="38" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>26</v>
@@ -4748,15 +4750,15 @@
         <v>193</v>
       </c>
       <c r="H67" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" s="38" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>26</v>
@@ -4777,15 +4779,15 @@
         <v>193</v>
       </c>
       <c r="H68" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>26</v>
@@ -4806,15 +4808,15 @@
         <v>193</v>
       </c>
       <c r="H69" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>26</v>
@@ -4835,15 +4837,15 @@
         <v>193</v>
       </c>
       <c r="H70" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>26</v>
@@ -4864,10 +4866,10 @@
         <v>193</v>
       </c>
       <c r="H71" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="144" x14ac:dyDescent="0.3">
@@ -4893,7 +4895,7 @@
         <v>193</v>
       </c>
       <c r="H72" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>212</v>
@@ -4922,10 +4924,10 @@
         <v>101</v>
       </c>
       <c r="H73" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -4951,10 +4953,10 @@
         <v>109</v>
       </c>
       <c r="H74" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I74" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -4980,10 +4982,10 @@
         <v>105</v>
       </c>
       <c r="H75" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.3">
@@ -5009,10 +5011,10 @@
         <v>107</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
@@ -5038,15 +5040,15 @@
         <v>103</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>26</v>
@@ -5067,10 +5069,10 @@
         <v>112</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
@@ -5096,10 +5098,10 @@
         <v>111</v>
       </c>
       <c r="H79" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
@@ -5119,16 +5121,16 @@
         <v>11</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>378</v>
+        <v>436</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>114</v>
       </c>
       <c r="H80" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
@@ -5154,7 +5156,7 @@
         <v>126</v>
       </c>
       <c r="H81" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>214</v>
@@ -5183,7 +5185,7 @@
         <v>34</v>
       </c>
       <c r="H82" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I82" s="14" t="s">
         <v>123</v>
@@ -5192,10 +5194,10 @@
     </row>
     <row r="83" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A83" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>122</v>
@@ -5213,19 +5215,19 @@
         <v>215</v>
       </c>
       <c r="H83" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>216</v>
+        <v>437</v>
       </c>
       <c r="J83" s="6"/>
     </row>
     <row r="84" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A84" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C84" s="16" t="s">
         <v>122</v>
@@ -5243,16 +5245,16 @@
         <v>215</v>
       </c>
       <c r="H84" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>222</v>
+        <v>438</v>
       </c>
       <c r="J84" s="6"/>
     </row>
     <row r="85" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>26</v>
@@ -5273,16 +5275,16 @@
         <v>215</v>
       </c>
       <c r="H85" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J85" s="6"/>
     </row>
     <row r="86" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A86" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>26</v>
@@ -5303,16 +5305,16 @@
         <v>215</v>
       </c>
       <c r="H86" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J86" s="6"/>
     </row>
     <row r="87" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A87" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>26</v>
@@ -5333,16 +5335,16 @@
         <v>215</v>
       </c>
       <c r="H87" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J87" s="6"/>
     </row>
     <row r="88" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>26</v>
@@ -5360,19 +5362,19 @@
         <v>41</v>
       </c>
       <c r="G88" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="H88" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I88" s="14" t="s">
         <v>255</v>
-      </c>
-      <c r="H88" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I88" s="14" t="s">
-        <v>257</v>
       </c>
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>26</v>
@@ -5390,43 +5392,43 @@
         <v>41</v>
       </c>
       <c r="G89" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H89" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J89" s="6"/>
     </row>
     <row r="90" spans="1:14" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A90" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" s="16" t="s">
+      <c r="H90" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I90" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="D90" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="H90" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I90" s="14" t="s">
-        <v>229</v>
       </c>
       <c r="J90" s="15"/>
       <c r="K90" s="15"/>
@@ -5436,13 +5438,13 @@
     </row>
     <row r="91" spans="1:14" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A91" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D91" s="16" t="s">
         <v>27</v>
@@ -5454,13 +5456,13 @@
         <v>11</v>
       </c>
       <c r="G91" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H91" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I91" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
@@ -5470,13 +5472,13 @@
     </row>
     <row r="92" spans="1:14" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A92" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D92" s="16" t="s">
         <v>27</v>
@@ -5488,13 +5490,13 @@
         <v>11</v>
       </c>
       <c r="G92" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H92" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I92" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J92" s="15"/>
       <c r="K92" s="15"/>
@@ -5510,7 +5512,7 @@
         <v>26</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D93" s="16" t="s">
         <v>27</v>
@@ -5525,10 +5527,10 @@
         <v>57</v>
       </c>
       <c r="H93" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I93" s="14" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J93" s="15"/>
       <c r="K93" s="15"/>
@@ -5559,7 +5561,7 @@
         <v>206</v>
       </c>
       <c r="H94" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I94" s="14" t="s">
         <v>207</v>
@@ -5588,7 +5590,7 @@
         <v>206</v>
       </c>
       <c r="H95" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I95" s="14" t="s">
         <v>210</v>
@@ -5617,7 +5619,7 @@
         <v>206</v>
       </c>
       <c r="H96" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I96" s="14" t="s">
         <v>208</v>
@@ -5625,7 +5627,7 @@
     </row>
     <row r="97" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A97" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>26</v>
@@ -5646,16 +5648,16 @@
         <v>126</v>
       </c>
       <c r="H97" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I97" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J97" s="6"/>
     </row>
     <row r="98" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>26</v>
@@ -5676,15 +5678,15 @@
         <v>64</v>
       </c>
       <c r="H98" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I98" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A99" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>26</v>
@@ -5705,15 +5707,15 @@
         <v>64</v>
       </c>
       <c r="H99" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I99" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A100" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>26</v>
@@ -5734,15 +5736,15 @@
         <v>64</v>
       </c>
       <c r="H100" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I100" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A101" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>26</v>
@@ -5763,10 +5765,10 @@
         <v>64</v>
       </c>
       <c r="H101" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I101" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
@@ -5792,10 +5794,10 @@
         <v>64</v>
       </c>
       <c r="H102" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I102" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -5821,10 +5823,10 @@
         <v>64</v>
       </c>
       <c r="H103" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -5850,15 +5852,15 @@
         <v>64</v>
       </c>
       <c r="H104" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I104" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>26</v>
@@ -5879,15 +5881,15 @@
         <v>64</v>
       </c>
       <c r="H105" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A106" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>26</v>
@@ -5908,15 +5910,15 @@
         <v>64</v>
       </c>
       <c r="H106" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I106" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A107" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>26</v>
@@ -5937,10 +5939,10 @@
         <v>64</v>
       </c>
       <c r="H107" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I107" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -5966,15 +5968,15 @@
         <v>64</v>
       </c>
       <c r="H108" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I108" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>26</v>
@@ -5995,10 +5997,10 @@
         <v>64</v>
       </c>
       <c r="H109" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I109" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -6024,7 +6026,7 @@
         <v>126</v>
       </c>
       <c r="H110" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>137</v>
@@ -6053,7 +6055,7 @@
         <v>126</v>
       </c>
       <c r="H111" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>127</v>
@@ -6061,7 +6063,7 @@
     </row>
     <row r="112" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A112" s="11" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>26</v>
@@ -6082,15 +6084,15 @@
         <v>126</v>
       </c>
       <c r="H112" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>26</v>
@@ -6108,18 +6110,18 @@
         <v>11</v>
       </c>
       <c r="G113" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H113" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I113" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="H113" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I113" s="14" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>26</v>
@@ -6137,21 +6139,21 @@
         <v>11</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H114" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I114" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>97</v>
@@ -6166,18 +6168,18 @@
         <v>11</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H115" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I115" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>26</v>
@@ -6195,18 +6197,18 @@
         <v>11</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H116" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I116" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>26</v>
@@ -6224,18 +6226,18 @@
         <v>11</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H117" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I117" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>26</v>
@@ -6253,13 +6255,13 @@
         <v>11</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H118" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I118" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -6285,7 +6287,7 @@
         <v>130</v>
       </c>
       <c r="H119" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I119" s="5" t="s">
         <v>131</v>
@@ -6314,7 +6316,7 @@
         <v>130</v>
       </c>
       <c r="H120" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>133</v>
@@ -6322,7 +6324,7 @@
     </row>
     <row r="121" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>26</v>
@@ -6343,15 +6345,15 @@
         <v>126</v>
       </c>
       <c r="H121" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>26</v>
@@ -6372,10 +6374,10 @@
         <v>126</v>
       </c>
       <c r="H122" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -6401,7 +6403,7 @@
         <v>135</v>
       </c>
       <c r="H123" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I123" s="14" t="s">
         <v>203</v>
@@ -6431,7 +6433,7 @@
         <v>30</v>
       </c>
       <c r="H124" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I124" s="14" t="s">
         <v>204</v>
@@ -6461,7 +6463,7 @@
         <v>32</v>
       </c>
       <c r="H125" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I125" s="14" t="s">
         <v>205</v>
@@ -6470,7 +6472,7 @@
     </row>
     <row r="126" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A126" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>26</v>
@@ -6488,19 +6490,19 @@
         <v>11</v>
       </c>
       <c r="G126" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H126" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I126" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J126" s="6"/>
     </row>
     <row r="127" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A127" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>26</v>
@@ -6518,19 +6520,19 @@
         <v>11</v>
       </c>
       <c r="G127" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H127" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I127" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J127" s="6"/>
     </row>
     <row r="128" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A128" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>26</v>
@@ -6548,19 +6550,19 @@
         <v>11</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H128" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I128" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J128" s="6"/>
     </row>
     <row r="129" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A129" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>26</v>
@@ -6578,19 +6580,19 @@
         <v>11</v>
       </c>
       <c r="G129" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H129" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I129" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J129" s="6"/>
     </row>
     <row r="130" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A130" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>26</v>
@@ -6608,19 +6610,19 @@
         <v>11</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H130" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I130" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J130" s="6"/>
     </row>
     <row r="131" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A131" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>26</v>
@@ -6638,19 +6640,19 @@
         <v>11</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H131" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I131" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J131" s="6"/>
     </row>
     <row r="132" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A132" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>26</v>
@@ -6668,19 +6670,19 @@
         <v>11</v>
       </c>
       <c r="G132" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H132" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I132" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J132" s="6"/>
     </row>
     <row r="133" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A133" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>26</v>
@@ -6698,19 +6700,19 @@
         <v>11</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H133" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I133" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J133" s="6"/>
     </row>
     <row r="134" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A134" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>26</v>
@@ -6728,25 +6730,25 @@
         <v>11</v>
       </c>
       <c r="G134" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H134" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I134" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J134" s="6"/>
     </row>
     <row r="135" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A135" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D135" s="16" t="s">
         <v>27</v>
@@ -6758,13 +6760,13 @@
         <v>11</v>
       </c>
       <c r="G135" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="H135" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I135" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="H135" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I135" s="14" t="s">
-        <v>246</v>
       </c>
       <c r="J135" s="6"/>
     </row>
@@ -6776,7 +6778,7 @@
         <v>26</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D136" s="16" t="s">
         <v>27</v>
@@ -6788,25 +6790,25 @@
         <v>11</v>
       </c>
       <c r="G136" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H136" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I136" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J136" s="6"/>
     </row>
     <row r="137" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A137" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>10</v>
@@ -6818,25 +6820,25 @@
         <v>41</v>
       </c>
       <c r="G137" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H137" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I137" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J137" s="6"/>
     </row>
     <row r="138" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A138" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>10</v>
@@ -6848,25 +6850,25 @@
         <v>41</v>
       </c>
       <c r="G138" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H138" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I138" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J138" s="6"/>
     </row>
     <row r="139" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A139" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D139" s="16" t="s">
         <v>27</v>
@@ -6878,25 +6880,25 @@
         <v>11</v>
       </c>
       <c r="G139" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H139" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I139" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J139" s="6"/>
     </row>
     <row r="140" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A140" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D140" s="16" t="s">
         <v>27</v>
@@ -6908,25 +6910,25 @@
         <v>11</v>
       </c>
       <c r="G140" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H140" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I140" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J140" s="6"/>
     </row>
     <row r="141" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A141" s="18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D141" s="16" t="s">
         <v>27</v>
@@ -6938,25 +6940,25 @@
         <v>11</v>
       </c>
       <c r="G141" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H141" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I141" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J141" s="6"/>
     </row>
     <row r="142" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A142" s="18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D142" s="16" t="s">
         <v>27</v>
@@ -6968,55 +6970,55 @@
         <v>11</v>
       </c>
       <c r="G142" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H142" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I142" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J142" s="6"/>
     </row>
     <row r="143" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A143" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="D143" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G143" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="H143" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I143" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D143" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E143" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F143" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G143" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="H143" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I143" s="14" t="s">
-        <v>250</v>
       </c>
       <c r="J143" s="6"/>
     </row>
     <row r="144" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A144" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C144" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D144" s="16" t="s">
         <v>27</v>
@@ -7028,25 +7030,25 @@
         <v>11</v>
       </c>
       <c r="G144" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H144" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I144" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J144" s="6"/>
     </row>
     <row r="145" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A145" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D145" s="16" t="s">
         <v>27</v>
@@ -7058,25 +7060,25 @@
         <v>11</v>
       </c>
       <c r="G145" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H145" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I145" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="J145" s="6"/>
     </row>
     <row r="146" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A146" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D146" s="16" t="s">
         <v>27</v>
@@ -7088,19 +7090,19 @@
         <v>11</v>
       </c>
       <c r="G146" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H146" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I146" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J146" s="6"/>
     </row>
     <row r="147" spans="1:13" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>26</v>
@@ -7121,10 +7123,10 @@
         <v>25</v>
       </c>
       <c r="H147" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I147" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J147" s="6"/>
       <c r="K147" s="6"/>
@@ -7133,7 +7135,7 @@
     </row>
     <row r="148" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>26</v>
@@ -7154,10 +7156,10 @@
         <v>25</v>
       </c>
       <c r="H148" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I148" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J148" s="6"/>
       <c r="K148" s="6"/>
@@ -7166,7 +7168,7 @@
     </row>
     <row r="149" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>26</v>
@@ -7187,10 +7189,10 @@
         <v>25</v>
       </c>
       <c r="H149" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I149" s="14" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="J149" s="6"/>
       <c r="K149" s="6"/>
@@ -7199,7 +7201,7 @@
     </row>
     <row r="150" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>26</v>
@@ -7220,10 +7222,10 @@
         <v>25</v>
       </c>
       <c r="H150" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I150" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J150" s="6"/>
       <c r="K150" s="6"/>
@@ -7232,7 +7234,7 @@
     </row>
     <row r="151" spans="1:13" ht="192" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>26</v>
@@ -7253,10 +7255,10 @@
         <v>25</v>
       </c>
       <c r="H151" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I151" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J151" s="6"/>
       <c r="K151" s="6"/>
@@ -7265,7 +7267,7 @@
     </row>
     <row r="152" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="30" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>26</v>
@@ -7283,13 +7285,13 @@
         <v>11</v>
       </c>
       <c r="G152" s="26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H152" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I152" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J152" s="24"/>
       <c r="K152" s="24"/>
@@ -7298,13 +7300,13 @@
     </row>
     <row r="153" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D153" s="26" t="s">
         <v>27</v>
@@ -7316,13 +7318,13 @@
         <v>11</v>
       </c>
       <c r="G153" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H153" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I153" s="37" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J153" s="24"/>
       <c r="K153" s="24"/>
@@ -7331,13 +7333,13 @@
     </row>
     <row r="154" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="30" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C154" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D154" s="26" t="s">
         <v>27</v>
@@ -7352,10 +7354,10 @@
         <v>105</v>
       </c>
       <c r="H154" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I154" s="37" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J154" s="24"/>
       <c r="K154" s="24"/>
@@ -7364,13 +7366,13 @@
     </row>
     <row r="155" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="30" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C155" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D155" s="26" t="s">
         <v>27</v>
@@ -7382,13 +7384,13 @@
         <v>11</v>
       </c>
       <c r="G155" s="26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H155" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I155" s="37" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="J155" s="24"/>
       <c r="K155" s="24"/>
@@ -7397,13 +7399,13 @@
     </row>
     <row r="156" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D156" s="16" t="s">
         <v>10</v>
@@ -7415,13 +7417,13 @@
         <v>19</v>
       </c>
       <c r="G156" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H156" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I156" s="37" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J156" s="24"/>
       <c r="K156" s="24"/>
@@ -7430,31 +7432,31 @@
     </row>
     <row r="157" spans="1:13" s="25" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>354</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="D157" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E157" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157" s="26" t="s">
         <v>356</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>357</v>
-      </c>
-      <c r="D157" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E157" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F157" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G157" s="26" t="s">
-        <v>358</v>
-      </c>
       <c r="H157" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I157" s="37" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J157" s="24"/>
       <c r="K157" s="24"/>
@@ -7463,31 +7465,31 @@
     </row>
     <row r="158" spans="1:13" s="25" customFormat="1" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>353</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C158" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C158" s="16" t="s">
+      <c r="D158" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E158" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F158" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G158" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="H158" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I158" s="37" t="s">
         <v>357</v>
-      </c>
-      <c r="D158" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E158" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F158" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G158" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="H158" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I158" s="37" t="s">
-        <v>359</v>
       </c>
       <c r="J158" s="24"/>
       <c r="K158" s="24"/>
@@ -7496,13 +7498,13 @@
     </row>
     <row r="159" spans="1:13" s="25" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D159" s="26" t="s">
         <v>27</v>
@@ -7514,13 +7516,13 @@
         <v>11</v>
       </c>
       <c r="G159" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="H159" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="I159" s="37" t="s">
         <v>358</v>
-      </c>
-      <c r="H159" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="I159" s="37" t="s">
-        <v>360</v>
       </c>
       <c r="J159" s="24"/>
       <c r="K159" s="24"/>
@@ -7529,13 +7531,13 @@
     </row>
     <row r="160" spans="1:13" s="25" customFormat="1" ht="187.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D160" s="16" t="s">
         <v>10</v>
@@ -7547,13 +7549,13 @@
         <v>19</v>
       </c>
       <c r="G160" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H160" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I160" s="37" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J160" s="24"/>
       <c r="K160" s="24"/>
@@ -7568,7 +7570,7 @@
         <v>26</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D161" s="16" t="s">
         <v>27</v>
@@ -7583,10 +7585,10 @@
         <v>43</v>
       </c>
       <c r="H161" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I161" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="J161" s="6"/>
       <c r="K161" s="6"/>
@@ -7601,7 +7603,7 @@
         <v>26</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D162" s="16" t="s">
         <v>27</v>
@@ -7616,10 +7618,10 @@
         <v>43</v>
       </c>
       <c r="H162" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I162" s="7" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J162" s="6"/>
       <c r="K162" s="6"/>
@@ -7634,7 +7636,7 @@
         <v>26</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D163" s="16" t="s">
         <v>10</v>
@@ -7643,16 +7645,16 @@
         <v>11</v>
       </c>
       <c r="F163" s="28" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G163" s="16" t="s">
         <v>43</v>
       </c>
       <c r="H163" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I163" s="7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J163" s="6"/>
       <c r="K163" s="6"/>
@@ -7667,7 +7669,7 @@
         <v>26</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D164" s="16" t="s">
         <v>10</v>
@@ -7676,16 +7678,16 @@
         <v>11</v>
       </c>
       <c r="F164" s="28" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G164" s="16" t="s">
         <v>43</v>
       </c>
       <c r="H164" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I164" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="J164" s="6"/>
       <c r="K164" s="6"/>
@@ -7700,7 +7702,7 @@
         <v>26</v>
       </c>
       <c r="C165" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D165" s="16" t="s">
         <v>27</v>
@@ -7715,10 +7717,10 @@
         <v>48</v>
       </c>
       <c r="H165" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I165" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="166" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -7729,7 +7731,7 @@
         <v>26</v>
       </c>
       <c r="C166" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D166" s="16" t="s">
         <v>27</v>
@@ -7744,10 +7746,10 @@
         <v>48</v>
       </c>
       <c r="H166" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I166" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="167" spans="1:13" ht="283.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7758,7 +7760,7 @@
         <v>26</v>
       </c>
       <c r="C167" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D167" s="16" t="s">
         <v>10</v>
@@ -7773,10 +7775,10 @@
         <v>69</v>
       </c>
       <c r="H167" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I167" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="168" spans="1:13" ht="204.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7787,7 +7789,7 @@
         <v>26</v>
       </c>
       <c r="C168" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D168" s="16" t="s">
         <v>10</v>
@@ -7802,10 +7804,10 @@
         <v>48</v>
       </c>
       <c r="H168" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I168" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
@@ -7816,7 +7818,7 @@
         <v>26</v>
       </c>
       <c r="C169" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D169" s="16" t="s">
         <v>10</v>
@@ -7831,10 +7833,10 @@
         <v>48</v>
       </c>
       <c r="H169" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I169" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="J169" s="6"/>
       <c r="K169" s="6"/>
@@ -7849,7 +7851,7 @@
         <v>26</v>
       </c>
       <c r="C170" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D170" s="16" t="s">
         <v>27</v>
@@ -7864,10 +7866,10 @@
         <v>48</v>
       </c>
       <c r="H170" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I170" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J170" s="6"/>
       <c r="K170" s="6"/>
@@ -7882,7 +7884,7 @@
         <v>26</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D171" s="16" t="s">
         <v>27</v>
@@ -7897,10 +7899,10 @@
         <v>48</v>
       </c>
       <c r="H171" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I171" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Scripts for Sanity Suite
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-merchant.xlsx
+++ b/Web/coyni/resources/TestScript-merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Merchant - Sanity Testing\clone_Merchant_sanity_27_12_2022\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56F1DAC-1CA1-4B6E-A8DA-2CBB47AB1BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A00025-6886-4659-8EFC-3E9D9B3136C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -359,11 +359,6 @@
     <t>Export Files</t>
   </si>
   <si>
-    <t>coyni.merchant.tests.TokenAccountTest,
-testExportFiles,
--pheading</t>
-  </si>
-  <si>
     <t>Verify merchant settings</t>
   </si>
   <si>
@@ -371,11 +366,6 @@
   </si>
   <si>
     <t>Merchant Settings</t>
-  </si>
-  <si>
-    <t>coyni.merchant.tests.MerchantSettingsTest,
-testMerchantSettingsLinks,
--pheading</t>
   </si>
   <si>
     <t>Verify Get Help</t>
@@ -392,9 +382,33 @@
 -pheading</t>
   </si>
   <si>
+    <t>coyni.merchant.tests.ExportFilesTest,
+testExportFiles,
+-pheading</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantSettingsTest,
+testMerchantSettingsLinks,
+-pheading,
+-pcompanyInformationHeading,
+-pdbaInformationHeading,
+-pbeneficiaryOwnersHeading,
+-ppaymentMethodsHeading,
+-ppreferencesHeading,
+-pagreementsHeading,
+-pfeesHeading,
+-paccountLimitsHeading,
+-pteamSharedHeading,
+-papiKeysHeading</t>
+  </si>
+  <si>
     <t>coyni.merchant.tests.MerchantProfileTest,
 testUserDetailsLinks,
--pheading</t>
+-pheading,
+-ppreferencesHeading,
+-pagreementsHeading,
+-pchangePasswordHeading,
+-ptwoStepAuthenticationHeading</t>
   </si>
 </sst>
 </file>
@@ -832,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +926,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -941,7 +955,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -971,7 +985,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>18</v>
@@ -1001,7 +1015,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>18</v>
@@ -1031,7 +1045,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>18</v>
@@ -1061,7 +1075,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>18</v>
@@ -1091,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>18</v>
@@ -1121,7 +1135,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>18</v>
@@ -1151,7 +1165,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>18</v>
@@ -1181,7 +1195,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>18</v>
@@ -1211,7 +1225,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1241,7 +1255,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>52</v>
@@ -1271,7 +1285,7 @@
         <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>52</v>
@@ -1301,7 +1315,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>52</v>
@@ -1331,7 +1345,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>18</v>
@@ -1364,7 +1378,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>44</v>
@@ -1397,7 +1411,7 @@
         <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -1455,7 +1469,7 @@
         <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>52</v>
@@ -1484,7 +1498,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>18</v>
@@ -1513,7 +1527,7 @@
         <v>70</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>71</v>
@@ -1534,65 +1548,65 @@
         <v>38</v>
       </c>
       <c r="I23" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="H24" s="10" t="s">
         <v>38</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="H25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Test scripts for Sanity Suite
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-merchant.xlsx
+++ b/Web/coyni/resources/TestScript-merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Merchant - Sanity Testing\clone_Merchant_sanity_27_12_2022\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A00025-6886-4659-8EFC-3E9D9B3136C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEAA2A0-C17D-42D1-9991-49473B5D45C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -338,11 +338,6 @@
     <t>Verify Merchant Activity Links</t>
   </si>
   <si>
-    <t>coyni.merchant.tests.MerchantActivityTest,
-testMerchantActivityLinks,
--pheading</t>
-  </si>
-  <si>
     <t>Verify Available Balance in Token Account</t>
   </si>
   <si>
@@ -409,6 +404,14 @@
 -pagreementsHeading,
 -pchangePasswordHeading,
 -ptwoStepAuthenticationHeading</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantActivityTest,
+testMerchantActivityLinks,
+-pheading,
+-ptransactionHeading,
+-ppayOutHistoryHeading,
+-preserveHistoryHeading</t>
   </si>
 </sst>
 </file>
@@ -846,26 +849,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="54.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.44140625" customWidth="1"/>
-    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="41.88671875" customWidth="1"/>
-    <col min="12" max="12" width="41.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.42578125" customWidth="1"/>
+    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="41.85546875" customWidth="1"/>
+    <col min="12" max="12" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -894,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="256.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="256.14999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>47</v>
       </c>
@@ -921,12 +924,12 @@
       </c>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:11" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -950,12 +953,12 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -980,12 +983,12 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>18</v>
@@ -1010,12 +1013,12 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>18</v>
@@ -1040,12 +1043,12 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>18</v>
@@ -1070,12 +1073,12 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>18</v>
@@ -1100,12 +1103,12 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>18</v>
@@ -1130,12 +1133,12 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>18</v>
@@ -1160,12 +1163,12 @@
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>18</v>
@@ -1190,12 +1193,12 @@
       </c>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>18</v>
@@ -1220,12 +1223,12 @@
       </c>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1250,12 +1253,12 @@
       </c>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>52</v>
@@ -1280,12 +1283,12 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>52</v>
@@ -1310,12 +1313,12 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>52</v>
@@ -1340,12 +1343,12 @@
       </c>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>18</v>
@@ -1373,12 +1376,12 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>44</v>
@@ -1406,12 +1409,12 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -1435,7 +1438,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1461,15 +1464,15 @@
         <v>38</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>52</v>
@@ -1490,15 +1493,15 @@
         <v>38</v>
       </c>
       <c r="I21" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>18</v>
@@ -1519,94 +1522,94 @@
         <v>38</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="H23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="10" t="s">
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="8" t="s">
+    <row r="25" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="D25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="H25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1642,12 +1645,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Modified Test Data and Test Script for Merchant Portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-merchant.xlsx
+++ b/Web/coyni/resources/TestScript-merchant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_web_2.3\clone_Merchant_2.3_24_04_2023\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_web_2.3\clone_Merchant_01_05_2023\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9A4D81-8302-4FFB-B252-5D71C5AB75B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F837E8-8760-4334-8C5C-FAF0ED7A408A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -2955,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6598,7 +6598,7 @@
         <v>153</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C114" s="16" t="s">
         <v>440</v>

</xml_diff>